<commit_message>
Tested two more photos
</commit_message>
<xml_diff>
--- a/eyeDetectionTestingLog.xlsx
+++ b/eyeDetectionTestingLog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Web Location</t>
   </si>
@@ -94,6 +94,20 @@
   </si>
   <si>
     <t>http://bloximages.chicago2.vip.townnews.com/azstarnet.com/content/tncms/assets/v3/editorial/3/78/3781cbf8-0d81-511b-8edd-10fcbf43ace5/50ef7ffaab184.preview-620.jpg</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Traceback (most recent call last):
+  File "C:\Users\Shannon\Documents\GitHub\DVS-Python\eyeDetection.py", line 99, in &lt;module&gt;
+    image = DetectRedEyes(img, faceCascade, eyeCascade)
+  File "C:\Users\Shannon\Documents\GitHub\DVS-Python\eyeDetection.py", line 71, in DetectRedEyes
+    cv.SetImageROI(image, (pt1[0],
+UnboundLocalError: local variable 'pt1' referenced before assignment</t>
   </si>
 </sst>
 </file>
@@ -469,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -516,9 +530,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="90">
+    <row r="3" spans="1:5" ht="210">
       <c r="A3" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="135">
@@ -586,24 +612,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="120">
+    <row r="17" spans="1:5" ht="120">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="90">
+    <row r="18" spans="1:5" ht="90">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="120">
+    <row r="19" spans="1:5" ht="120">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="75">
+    <row r="20" spans="1:5" ht="75">
       <c r="A20" s="5" t="s">
         <v>24</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tested all photos on log
</commit_message>
<xml_diff>
--- a/eyeDetectionTestingLog.xlsx
+++ b/eyeDetectionTestingLog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
   <si>
     <t>Web Location</t>
   </si>
@@ -108,6 +108,36 @@
   File "C:\Users\Shannon\Documents\GitHub\DVS-Python\eyeDetection.py", line 71, in DetectRedEyes
     cv.SetImageROI(image, (pt1[0],
 UnboundLocalError: local variable 'pt1' referenced before assignment</t>
+  </si>
+  <si>
+    <t>Nostril and right ear falsely recognized</t>
+  </si>
+  <si>
+    <t>Some false recognition on left forehead. Picture is too large to see the rest of and cannot be scrolled across or resized</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Cannot see eyes because window can't be resized</t>
+  </si>
+  <si>
+    <t>Left eye double selected</t>
+  </si>
+  <si>
+    <t>Doesn't even recognize the face correctly</t>
+  </si>
+  <si>
+    <t>Falsely recognizes left nostril</t>
+  </si>
+  <si>
+    <t>Does not recognize eyes</t>
+  </si>
+  <si>
+    <t>Double selects left eye, does not select right eye</t>
+  </si>
+  <si>
+    <t>Does not capture full right eye</t>
   </si>
 </sst>
 </file>
@@ -481,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -551,96 +581,271 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="135">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="105">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="105">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="75">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="75">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="75">
-      <c r="A10" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="75">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="135">
       <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="135">
-      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="120">
-      <c r="A13" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="120">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="90">
-      <c r="A14" s="1" t="s">
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="90">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="60">
-      <c r="A15" s="1" t="s">
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="195">
-      <c r="A16" s="1" t="s">
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="195">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="120">
-      <c r="A17" s="5" t="s">
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="210">
+      <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="90">
-      <c r="A18" s="1" t="s">
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="90">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="120">
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="120">
+      <c r="A18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="75">
       <c r="A19" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="75">
-      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="4">
-        <v>41389</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="D19" s="4">
+        <v>41389</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -653,14 +858,19 @@
     <hyperlink ref="A7" r:id="rId5"/>
     <hyperlink ref="A8" r:id="rId6"/>
     <hyperlink ref="A9" r:id="rId7"/>
-    <hyperlink ref="A10" r:id="rId8"/>
-    <hyperlink ref="A17" r:id="rId9"/>
+    <hyperlink ref="A16" r:id="rId8"/>
+    <hyperlink ref="A18" r:id="rId9"/>
     <hyperlink ref="A19" r:id="rId10"/>
-    <hyperlink ref="A20" r:id="rId11"/>
-    <hyperlink ref="A2" r:id="rId12"/>
+    <hyperlink ref="A2" r:id="rId11"/>
+    <hyperlink ref="A10" r:id="rId12"/>
+    <hyperlink ref="A12" r:id="rId13"/>
+    <hyperlink ref="A13" r:id="rId14"/>
+    <hyperlink ref="A14" r:id="rId15"/>
+    <hyperlink ref="A15" r:id="rId16"/>
+    <hyperlink ref="A17" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
tested a new photo
</commit_message>
<xml_diff>
--- a/eyeDetectionTestingLog.xlsx
+++ b/eyeDetectionTestingLog.xlsx
@@ -15,8 +15,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Shannon</author>
+  </authors>
+  <commentList>
+    <comment ref="A20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shannon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>Web Location</t>
   </si>
@@ -139,12 +173,18 @@
   <si>
     <t>Does not capture full right eye</t>
   </si>
+  <si>
+    <t>http://babelhofer.files.wordpress.com/2010/06/asian-baby.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nostril selected </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +206,19 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -511,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -846,6 +899,23 @@
         <v>41389</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="75">
+      <c r="A20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="4">
+        <v>41391</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -868,9 +938,11 @@
     <hyperlink ref="A14" r:id="rId15"/>
     <hyperlink ref="A15" r:id="rId16"/>
     <hyperlink ref="A17" r:id="rId17"/>
+    <hyperlink ref="A20" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>